<commit_message>
Update info/RASM arduino Mega pin table.xlsx
</commit_message>
<xml_diff>
--- a/info/RASM arduino Mega pin table.xlsx
+++ b/info/RASM arduino Mega pin table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7935" windowHeight="6390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7935" windowHeight="6390" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PIN INFORMATION" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="25">
   <si>
     <t>pin #s</t>
   </si>
@@ -77,6 +77,30 @@
   </si>
   <si>
     <t>M2SF</t>
+  </si>
+  <si>
+    <t>MOTOR SHIELD 2</t>
+  </si>
+  <si>
+    <t>MOTOR SHIELD 3</t>
+  </si>
+  <si>
+    <t>ENCODER 1</t>
+  </si>
+  <si>
+    <t>ENCODER 2</t>
+  </si>
+  <si>
+    <t>ENCODER 3</t>
+  </si>
+  <si>
+    <t>ENCODER 4</t>
+  </si>
+  <si>
+    <t>ENCODER 5</t>
+  </si>
+  <si>
+    <t>ENCODER 6</t>
   </si>
 </sst>
 </file>
@@ -99,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +142,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -128,12 +164,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -161,9 +199,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="1" builtinId="47"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -445,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -459,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1044,12 +1096,688 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="14">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="14">
+        <v>9</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2">
+        <v>23</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2">
+        <v>25</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>27</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>28</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5">
+        <v>30</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5">
+        <v>31</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5">
+        <v>32</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="5">
+        <v>33</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="5">
+        <v>34</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="5">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="12">
+        <v>36</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="12">
+        <v>37</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="12">
+        <v>38</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="12">
+        <v>39</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="12">
+        <v>40</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="12">
+        <v>41</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="13">
+        <v>42</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="13">
+        <v>43</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="13">
+        <v>44</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="13">
+        <v>45</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="13">
+        <v>46</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="13">
+        <v>47</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>48</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>49</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>50</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="2">
+        <v>51</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
+        <v>52</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="2">
+        <v>53</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>